<commit_message>
added pictures of initial and current design-edited presentation
</commit_message>
<xml_diff>
--- a/MajorProject/planning/PDE3400 budget.xlsx
+++ b/MajorProject/planning/PDE3400 budget.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19126"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marlon Gwira\Desktop\MajorProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marlon Gwira\MobileRobotRos_finalYearProject\MajorProject\planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01293C93-CD34-47A4-BB8B-63D746872953}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="240" windowWidth="20235" windowHeight="14655" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="179017" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -612,6 +613,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -635,36 +666,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
@@ -1016,8 +1017,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:G2"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1029,159 +1030,159 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
     </row>
     <row r="2" spans="1:7" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="28"/>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
+      <c r="A2" s="38"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
     </row>
     <row r="3" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="31"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="41"/>
     </row>
     <row r="4" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A4" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="33"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="43"/>
     </row>
     <row r="5" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A5" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="32" t="s">
+      <c r="B5" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="32"/>
-      <c r="D5" s="32"/>
-      <c r="E5" s="32"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="33"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="43"/>
     </row>
     <row r="6" spans="1:7" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="34"/>
-      <c r="D6" s="34"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="34"/>
-      <c r="G6" s="35"/>
+      <c r="C6" s="44"/>
+      <c r="D6" s="44"/>
+      <c r="E6" s="44"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="45"/>
     </row>
     <row r="7" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="29"/>
-      <c r="B7" s="29"/>
-      <c r="C7" s="29"/>
-      <c r="D7" s="29"/>
-      <c r="E7" s="29"/>
-      <c r="F7" s="29"/>
-      <c r="G7" s="29"/>
+      <c r="A7" s="39"/>
+      <c r="B7" s="39"/>
+      <c r="C7" s="39"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="39"/>
+      <c r="G7" s="39"/>
     </row>
     <row r="8" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A8" s="36" t="s">
+      <c r="A8" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="37"/>
-      <c r="C8" s="37"/>
-      <c r="D8" s="37"/>
-      <c r="E8" s="37"/>
-      <c r="F8" s="37"/>
-      <c r="G8" s="38"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="31"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
-      <c r="B9" s="39" t="s">
+      <c r="B9" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="40"/>
-      <c r="D9" s="40"/>
-      <c r="E9" s="40"/>
-      <c r="F9" s="40"/>
-      <c r="G9" s="41"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="34"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="42" t="s">
+      <c r="B10" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="C10" s="43"/>
-      <c r="D10" s="43"/>
-      <c r="E10" s="43"/>
-      <c r="F10" s="43"/>
-      <c r="G10" s="44"/>
+      <c r="C10" s="36"/>
+      <c r="D10" s="36"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
+      <c r="G10" s="37"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="42" t="s">
+      <c r="B11" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="C11" s="43"/>
-      <c r="D11" s="43"/>
-      <c r="E11" s="43"/>
-      <c r="F11" s="43"/>
-      <c r="G11" s="44"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="37"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="42" t="s">
+      <c r="B12" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="C12" s="43"/>
-      <c r="D12" s="43"/>
-      <c r="E12" s="43"/>
-      <c r="F12" s="43"/>
-      <c r="G12" s="44"/>
+      <c r="C12" s="36"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="36"/>
+      <c r="G12" s="37"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="42" t="s">
+      <c r="B13" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="C13" s="43"/>
-      <c r="D13" s="43"/>
-      <c r="E13" s="43"/>
-      <c r="F13" s="43"/>
-      <c r="G13" s="44"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="36"/>
+      <c r="G13" s="37"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
@@ -1213,25 +1214,25 @@
       <c r="A16" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B16" s="42" t="s">
+      <c r="B16" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="C16" s="43"/>
-      <c r="D16" s="43"/>
-      <c r="E16" s="43"/>
-      <c r="F16" s="43"/>
-      <c r="G16" s="44"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="36"/>
+      <c r="G16" s="37"/>
     </row>
     <row r="17" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A17" s="36" t="s">
+      <c r="A17" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="37"/>
-      <c r="C17" s="37"/>
-      <c r="D17" s="37"/>
-      <c r="E17" s="37"/>
-      <c r="F17" s="37"/>
-      <c r="G17" s="38"/>
+      <c r="B17" s="30"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="31"/>
     </row>
     <row r="18" spans="1:7" ht="45.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
@@ -1604,6 +1605,13 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A7:G7"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B6:G6"/>
     <mergeCell ref="A17:G17"/>
     <mergeCell ref="A8:G8"/>
     <mergeCell ref="B9:G9"/>
@@ -1612,13 +1620,6 @@
     <mergeCell ref="B12:G12"/>
     <mergeCell ref="B13:G13"/>
     <mergeCell ref="B16:G16"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A7:G7"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B6:G6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B20" r:id="rId1" xr:uid="{43C53D9F-D6C4-431B-8024-ED06090A7A73}"/>

</xml_diff>